<commit_message>
Corrected incorrect mapping for apnCrmLeadUniqueIdentifier
`apnCrmLeadUniqueIdentifier` is incorrectly mapped to `PartnerOpportunityIdentifier` and the Field Name - ACE Pipeline Manager2 column value is missing for this mapping on the documentation page.
</commit_message>
<xml_diff>
--- a/partner-central-apis/MappingToS3Fields.xlsx
+++ b/partner-central-apis/MappingToS3Fields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksmenon/Documents/CRMDocs/partner-crm-integration-samples/partner-central-apis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81FF258-0678-4246-80C6-034258B7945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE113B78-08BC-DC4A-9BD4-1C5C21D28447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38920" yWindow="-33340" windowWidth="30080" windowHeight="31640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -948,13 +948,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1301,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1987,7 +1987,7 @@
         <v>58</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>